<commit_message>
Update Schwall_Gayathri_Timesheet_october_2021 - Copy - Copy.xlsx
</commit_message>
<xml_diff>
--- a/Gayathri/Timesheet/Schwall_Gayathri_Timesheet_october_2021 - Copy - Copy.xlsx
+++ b/Gayathri/Timesheet/Schwall_Gayathri_Timesheet_october_2021 - Copy - Copy.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBFF6A8F-42DD-426A-8DA3-159FC67C7D24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2080B875-2BE9-4322-A259-6C1C2A40E26D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
   <si>
     <t>SlNo</t>
   </si>
@@ -48,6 +48,18 @@
   </si>
   <si>
     <t>onboarding employ workflow</t>
+  </si>
+  <si>
+    <t>interview question</t>
+  </si>
+  <si>
+    <t>java</t>
+  </si>
+  <si>
+    <t>Meeting</t>
+  </si>
+  <si>
+    <t>java ms refresher course</t>
   </si>
 </sst>
 </file>
@@ -551,7 +563,7 @@
   <dimension ref="B1:F145"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -619,18 +631,34 @@
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B6" s="2"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="3"/>
+      <c r="B6" s="2">
+        <v>2</v>
+      </c>
+      <c r="C6" s="10">
+        <v>44473</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="3">
+        <v>3</v>
+      </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7" s="2"/>
       <c r="C7" s="10"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="3"/>
+      <c r="D7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8" s="2"/>

</xml_diff>